<commit_message>
Cleaned up rows and notes in ground truth validation set
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_validation_set.xlsx
+++ b/GHT/ground_truth_detection_pts_validation_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490DE53D-15A8-40FA-AC80-50D0D1CA5581}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56C7B98-2EF7-414B-8ECD-2099D4557C54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A37" sqref="A32:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1853,18 +1853,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="2">
-        <v>9189512</v>
-      </c>
-      <c r="B102">
-        <v>37</v>
-      </c>
-      <c r="C102">
-        <v>57</v>
-      </c>
-      <c r="D102">
-        <v>26</v>
-      </c>
+      <c r="A102" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F102">

</xml_diff>

<commit_message>
Addition of Standard Deviations and Means
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_validation_set.xlsx
+++ b/GHT/ground_truth_detection_pts_validation_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74994245-411D-46A3-B5CD-9EA6CA0A3977}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84A9594-4020-48D7-88DB-2BCC1B258747}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Ground Truth Points" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -61,6 +62,15 @@
   </si>
   <si>
     <t>Sigma_z</t>
+  </si>
+  <si>
+    <t>Mean_x</t>
+  </si>
+  <si>
+    <t>Mean_y</t>
+  </si>
+  <si>
+    <t>Mean_z</t>
   </si>
 </sst>
 </file>
@@ -433,20 +443,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="54.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="2" max="4" width="6.59765625" customWidth="1"/>
+    <col min="5" max="5" width="54.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -455,7 +465,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,8 +490,17 @@
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>4491140</v>
       </c>
@@ -496,19 +515,31 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3">
-        <f>STDEV(B3:B102)</f>
-        <v>5.3482650826169165</v>
+        <f>STDEVP(B3:B102)</f>
+        <v>5.2501809492626057</v>
       </c>
       <c r="G3">
-        <f>STDEV(C3:C102)</f>
-        <v>8.7521368242217932</v>
+        <f>STDEVP(C3:C102)</f>
+        <v>8.7082661879389054</v>
       </c>
       <c r="H3">
-        <f>STDEV(D3:D102)</f>
-        <v>3.2749277114390667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <f>STDEVP(D3:D102)</f>
+        <v>3.3022870862479534</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(B3:B102)</f>
+        <v>29.66</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE(C3:C102)</f>
+        <v>51.69</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(D3:D102)</f>
+        <v>20.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>4687879</v>
       </c>
@@ -519,10 +550,10 @@
         <v>33</v>
       </c>
       <c r="D4" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4697342</v>
       </c>
@@ -536,7 +567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>4737315</v>
       </c>
@@ -550,7 +581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>4831559</v>
       </c>
@@ -564,7 +595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>4930402</v>
       </c>
@@ -578,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>5056218</v>
       </c>
@@ -592,7 +623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>5103832</v>
       </c>
@@ -606,7 +637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>5131203</v>
       </c>
@@ -620,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>5199556</v>
       </c>
@@ -634,7 +665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>5235783</v>
       </c>
@@ -645,10 +676,10 @@
         <v>59</v>
       </c>
       <c r="D13" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>5334421</v>
       </c>
@@ -662,7 +693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>5372580</v>
       </c>
@@ -673,10 +704,10 @@
         <v>54</v>
       </c>
       <c r="D15" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>5411573</v>
       </c>
@@ -690,7 +721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>5433681</v>
       </c>
@@ -704,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>5506328</v>
       </c>
@@ -721,7 +752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>5523521</v>
       </c>
@@ -735,7 +766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>5544945</v>
       </c>
@@ -749,7 +780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>5680178</v>
       </c>
@@ -763,7 +794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>5739421</v>
       </c>
@@ -777,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>5826444</v>
       </c>
@@ -791,7 +822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>5835023</v>
       </c>
@@ -802,10 +833,10 @@
         <v>64</v>
       </c>
       <c r="D24" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>6022046</v>
       </c>
@@ -819,7 +850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>6029287</v>
       </c>
@@ -833,7 +864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>6067977</v>
       </c>
@@ -847,12 +878,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>6095054</v>
       </c>
       <c r="B28" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2">
         <v>47</v>
@@ -861,21 +892,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>6173842</v>
       </c>
       <c r="B29" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2">
         <v>58</v>
       </c>
       <c r="D29" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>6201211</v>
       </c>
@@ -889,7 +920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>6218246</v>
       </c>
@@ -903,7 +934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>6268647</v>
       </c>
@@ -914,10 +945,10 @@
         <v>48</v>
       </c>
       <c r="D32" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>6490491</v>
       </c>
@@ -931,7 +962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>6729799</v>
       </c>
@@ -945,7 +976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>6828936</v>
       </c>
@@ -959,7 +990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>6868398</v>
       </c>
@@ -973,7 +1004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>6881614</v>
       </c>
@@ -987,7 +1018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>6993961</v>
       </c>
@@ -1001,7 +1032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>7081341</v>
       </c>
@@ -1012,10 +1043,10 @@
         <v>53</v>
       </c>
       <c r="D39" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>7222303</v>
       </c>
@@ -1029,7 +1060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>7257259</v>
       </c>
@@ -1043,7 +1074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>7299268</v>
       </c>
@@ -1057,7 +1088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>7316415</v>
       </c>
@@ -1071,7 +1102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>7337296</v>
       </c>
@@ -1085,7 +1116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>7396455</v>
       </c>
@@ -1096,10 +1127,10 @@
         <v>56</v>
       </c>
       <c r="D45" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>7444276</v>
       </c>
@@ -1113,7 +1144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>7466141</v>
       </c>
@@ -1127,7 +1158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>7489680</v>
       </c>
@@ -1141,7 +1172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>7496249</v>
       </c>
@@ -1155,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>7499820</v>
       </c>
@@ -1169,7 +1200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>7629097</v>
       </c>
@@ -1183,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>7796800</v>
       </c>
@@ -1197,7 +1228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>7800424</v>
       </c>
@@ -1211,7 +1242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>7887075</v>
       </c>
@@ -1225,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>7958084</v>
       </c>
@@ -1239,7 +1270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>7962433</v>
       </c>
@@ -1253,7 +1284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>8108990</v>
       </c>
@@ -1267,7 +1298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>8214092</v>
       </c>
@@ -1281,7 +1312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>8280387</v>
       </c>
@@ -1295,7 +1326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>8285119</v>
       </c>
@@ -1309,7 +1340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>8399974</v>
       </c>
@@ -1323,7 +1354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>8412228</v>
       </c>
@@ -1337,7 +1368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>8417665</v>
       </c>
@@ -1351,7 +1382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>8419199</v>
       </c>
@@ -1365,7 +1396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>8437096</v>
       </c>
@@ -1379,7 +1410,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>8441021</v>
       </c>
@@ -1393,7 +1424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>8476267</v>
       </c>
@@ -1407,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>8509076</v>
       </c>
@@ -1421,7 +1452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>8512802</v>
       </c>
@@ -1435,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>8540998</v>
       </c>
@@ -1449,7 +1480,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>8578004</v>
       </c>
@@ -1460,10 +1491,10 @@
         <v>55</v>
       </c>
       <c r="D71">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>8609486</v>
       </c>
@@ -1477,7 +1508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>8649024</v>
       </c>
@@ -1488,10 +1519,10 @@
         <v>32</v>
       </c>
       <c r="D73">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>8649140</v>
       </c>
@@ -1505,7 +1536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>8664266</v>
       </c>
@@ -1519,7 +1550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>8666303</v>
       </c>
@@ -1533,7 +1564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>8687072</v>
       </c>
@@ -1547,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>8697536</v>
       </c>
@@ -1561,7 +1592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>8717421</v>
       </c>
@@ -1575,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>8723551</v>
       </c>
@@ -1589,7 +1620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>8734298</v>
       </c>
@@ -1603,7 +1634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>8766117</v>
       </c>
@@ -1617,7 +1648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>8791550</v>
       </c>
@@ -1631,7 +1662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>8837927</v>
       </c>
@@ -1645,7 +1676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>8847103</v>
       </c>
@@ -1659,7 +1690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>8864910</v>
       </c>
@@ -1673,7 +1704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>8920727</v>
       </c>
@@ -1687,7 +1718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>8931170</v>
       </c>
@@ -1701,7 +1732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>8931305</v>
       </c>
@@ -1715,7 +1746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>8958140</v>
       </c>
@@ -1729,7 +1760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>8976584</v>
       </c>
@@ -1743,7 +1774,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>9014200</v>
       </c>
@@ -1757,7 +1788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>9020776</v>
       </c>
@@ -1771,7 +1802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>9043600</v>
       </c>
@@ -1785,7 +1816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>9049401</v>
       </c>
@@ -1799,7 +1830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>9063971</v>
       </c>
@@ -1813,7 +1844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>9086188</v>
       </c>
@@ -1827,7 +1858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>9115352</v>
       </c>
@@ -1841,7 +1872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>9118382</v>
       </c>
@@ -1855,7 +1886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>9136320</v>
       </c>
@@ -1869,7 +1900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>9145963</v>
       </c>
@@ -1883,7 +1914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>9189512</v>
       </c>

</xml_diff>

<commit_message>
Added distribution charts for empirical prior
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_validation_set.xlsx
+++ b/GHT/ground_truth_detection_pts_validation_set.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84A9594-4020-48D7-88DB-2BCC1B258747}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D621CE-6C8E-41C5-A9EE-62A204285AB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ground Truth Points" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Ground Truth Points'!$B$3:$B$102</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -144,6 +149,1387 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution of X-Points for Ground Truth</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Distribution of X-Points for Ground Truth</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{E5A034D4-2494-4C03-84A8-10B9421FE529}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution of Y-Points for Ground Truth</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Distribution of Y-Points for Ground Truth</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{DE3048D2-95D4-4A28-84E1-7BA8B6855EC8}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="4"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2214561</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>550857</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1581</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A4A8D3-D213-41F6-ACD8-67C3A059A536}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4665661" y="806444"/>
+              <a:ext cx="4851396" cy="2509837"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2208205</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>179380</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871BF5D0-2362-4C20-BE0B-8069ABF215F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4659305" y="3479793"/>
+              <a:ext cx="4878394" cy="2592387"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,7 +1832,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1937,5 +3323,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest version of GHT.py with some bugs regarding number of scans taken to generate histogram
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_validation_set.xlsx
+++ b/GHT/ground_truth_detection_pts_validation_set.xlsx
@@ -5,23 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D621CE-6C8E-41C5-A9EE-62A204285AB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BCB02C-CE23-41B9-92B2-40D158E17559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
+    <workbookView xWindow="10410" yWindow="1190" windowWidth="24220" windowHeight="17910" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ground Truth Points" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Ground Truth Points'!$B$3:$B$102</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Ground Truth Points'!$B$3:$B$102</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Ground Truth Points'!$M$25</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Ground Truth Points'!$N$25</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Ground Truth Points'!$M$25</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Ground Truth Points'!$N$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -151,12 +158,665 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Probability</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Surrounding Detected Point vs Scaled Accumulator Matrix Value</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ground Truth Points'!$N$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ground Truth Points'!$M$26:$M$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ground Truth Points'!$N$26:$N$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.7639751552795004E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.3333333333333297E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2797858099062903E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.0089686098654699E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.12234706616729001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.207792207792207</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.216911764705882</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.35820895522388002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.57692307692307598</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.72727272727272696</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A04-47EC-9ADE-5110B8388317}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="478613304"/>
+        <c:axId val="478611664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="478613304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="35"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Scaled</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Accumulator Matrix Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478611664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="478611664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Around Detected Pt/ Total #</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478613304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -355,6 +1015,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -1367,6 +2067,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1420,8 +2636,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4665661" y="806444"/>
-              <a:ext cx="4851396" cy="2509837"/>
+              <a:off x="4627561" y="806444"/>
+              <a:ext cx="4610096" cy="2509837"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1498,8 +2714,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4659305" y="3479793"/>
-              <a:ext cx="4878394" cy="2592387"/>
+              <a:off x="4621205" y="3479793"/>
+              <a:ext cx="4637094" cy="2592387"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1527,6 +2743,42 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1489074</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330199</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>44449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{019FE61B-2800-414B-B79D-8251B3EAD91E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1829,20 +3081,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="4" width="6.59765625" customWidth="1"/>
-    <col min="5" max="5" width="54.9296875" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
+    <col min="2" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="54.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1851,7 +3103,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +3138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>4491140</v>
       </c>
@@ -1925,7 +3177,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>4687879</v>
       </c>
@@ -1939,7 +3191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4697342</v>
       </c>
@@ -1953,7 +3205,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4737315</v>
       </c>
@@ -1967,7 +3219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4831559</v>
       </c>
@@ -1981,7 +3233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4930402</v>
       </c>
@@ -1995,7 +3247,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>5056218</v>
       </c>
@@ -2009,7 +3261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>5103832</v>
       </c>
@@ -2023,7 +3275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>5131203</v>
       </c>
@@ -2037,7 +3289,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>5199556</v>
       </c>
@@ -2051,7 +3303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>5235783</v>
       </c>
@@ -2065,7 +3317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>5334421</v>
       </c>
@@ -2079,7 +3331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>5372580</v>
       </c>
@@ -2093,7 +3345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>5411573</v>
       </c>
@@ -2107,7 +3359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>5433681</v>
       </c>
@@ -2121,7 +3373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>5506328</v>
       </c>
@@ -2138,7 +3390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>5523521</v>
       </c>
@@ -2152,7 +3404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>5544945</v>
       </c>
@@ -2166,7 +3418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>5680178</v>
       </c>
@@ -2180,7 +3432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>5739421</v>
       </c>
@@ -2194,7 +3446,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>5826444</v>
       </c>
@@ -2208,7 +3460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>5835023</v>
       </c>
@@ -2222,7 +3474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>6022046</v>
       </c>
@@ -2235,8 +3487,14 @@
       <c r="D25" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M25" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>6029287</v>
       </c>
@@ -2249,8 +3507,14 @@
       <c r="D26" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>6067977</v>
       </c>
@@ -2263,8 +3527,14 @@
       <c r="D27" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>6095054</v>
       </c>
@@ -2277,8 +3547,14 @@
       <c r="D28" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>6173842</v>
       </c>
@@ -2291,8 +3567,14 @@
       <c r="D29" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>6201211</v>
       </c>
@@ -2305,8 +3587,14 @@
       <c r="D30" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>6218246</v>
       </c>
@@ -2319,8 +3607,14 @@
       <c r="D31" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="M31">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>6268647</v>
       </c>
@@ -2333,8 +3627,14 @@
       <c r="D32" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>6490491</v>
       </c>
@@ -2347,8 +3647,14 @@
       <c r="D33" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M33">
+        <v>7</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>6729799</v>
       </c>
@@ -2361,8 +3667,14 @@
       <c r="D34" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M34">
+        <v>8</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>6828936</v>
       </c>
@@ -2375,8 +3687,14 @@
       <c r="D35" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M35">
+        <v>9</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>6868398</v>
       </c>
@@ -2389,8 +3707,14 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>6881614</v>
       </c>
@@ -2403,8 +3727,14 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M37">
+        <v>11</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>6993961</v>
       </c>
@@ -2417,8 +3747,14 @@
       <c r="D38" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M38">
+        <v>12</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>7081341</v>
       </c>
@@ -2431,8 +3767,14 @@
       <c r="D39" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M39">
+        <v>13</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>7222303</v>
       </c>
@@ -2445,8 +3787,14 @@
       <c r="D40" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M40">
+        <v>14</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>7257259</v>
       </c>
@@ -2459,8 +3807,14 @@
       <c r="D41" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M41">
+        <v>15</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>7299268</v>
       </c>
@@ -2473,8 +3827,14 @@
       <c r="D42" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M42">
+        <v>16</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>7316415</v>
       </c>
@@ -2487,8 +3847,14 @@
       <c r="D43" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M43">
+        <v>17</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>7337296</v>
       </c>
@@ -2501,8 +3867,14 @@
       <c r="D44" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M44">
+        <v>18</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>7396455</v>
       </c>
@@ -2515,8 +3887,14 @@
       <c r="D45" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M45">
+        <v>19</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>7444276</v>
       </c>
@@ -2529,8 +3907,14 @@
       <c r="D46" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M46">
+        <v>20</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>7466141</v>
       </c>
@@ -2543,8 +3927,14 @@
       <c r="D47" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M47">
+        <v>21</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>7489680</v>
       </c>
@@ -2557,8 +3947,14 @@
       <c r="D48" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M48">
+        <v>22</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>7496249</v>
       </c>
@@ -2571,8 +3967,14 @@
       <c r="D49" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M49">
+        <v>23</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>7499820</v>
       </c>
@@ -2585,8 +3987,14 @@
       <c r="D50" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M50">
+        <v>24</v>
+      </c>
+      <c r="N50">
+        <v>7.7639751552795004E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>7629097</v>
       </c>
@@ -2599,8 +4007,14 @@
       <c r="D51" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M51">
+        <v>25</v>
+      </c>
+      <c r="N51">
+        <v>8.3333333333333297E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>7796800</v>
       </c>
@@ -2613,8 +4027,14 @@
       <c r="D52" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M52">
+        <v>26</v>
+      </c>
+      <c r="N52">
+        <v>3.2797858099062903E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>7800424</v>
       </c>
@@ -2627,8 +4047,14 @@
       <c r="D53" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M53">
+        <v>27</v>
+      </c>
+      <c r="N53">
+        <v>6.0089686098654699E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>7887075</v>
       </c>
@@ -2641,8 +4067,14 @@
       <c r="D54" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M54">
+        <v>28</v>
+      </c>
+      <c r="N54">
+        <v>0.12234706616729001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>7958084</v>
       </c>
@@ -2655,8 +4087,14 @@
       <c r="D55" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M55">
+        <v>29</v>
+      </c>
+      <c r="N55">
+        <v>0.207792207792207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>7962433</v>
       </c>
@@ -2669,8 +4107,14 @@
       <c r="D56" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M56">
+        <v>30</v>
+      </c>
+      <c r="N56">
+        <v>0.216911764705882</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>8108990</v>
       </c>
@@ -2683,8 +4127,14 @@
       <c r="D57">
         <v>21</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M57">
+        <v>31</v>
+      </c>
+      <c r="N57">
+        <v>0.35820895522388002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>8214092</v>
       </c>
@@ -2697,8 +4147,14 @@
       <c r="D58">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M58">
+        <v>32</v>
+      </c>
+      <c r="N58">
+        <v>0.57692307692307598</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>8280387</v>
       </c>
@@ -2711,8 +4167,14 @@
       <c r="D59">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M59">
+        <v>33</v>
+      </c>
+      <c r="N59">
+        <v>0.72727272727272696</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>8285119</v>
       </c>
@@ -2725,8 +4187,14 @@
       <c r="D60">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="M60">
+        <v>34</v>
+      </c>
+      <c r="N60">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>8399974</v>
       </c>
@@ -2740,7 +4208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>8412228</v>
       </c>
@@ -2754,7 +4222,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>8417665</v>
       </c>
@@ -2768,7 +4236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>8419199</v>
       </c>
@@ -2782,7 +4250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>8437096</v>
       </c>
@@ -2796,7 +4264,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>8441021</v>
       </c>
@@ -2810,7 +4278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>8476267</v>
       </c>
@@ -2824,7 +4292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>8509076</v>
       </c>
@@ -2838,7 +4306,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>8512802</v>
       </c>
@@ -2852,7 +4320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>8540998</v>
       </c>
@@ -2866,7 +4334,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>8578004</v>
       </c>
@@ -2880,7 +4348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>8609486</v>
       </c>
@@ -2894,7 +4362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>8649024</v>
       </c>
@@ -2908,7 +4376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>8649140</v>
       </c>
@@ -2922,7 +4390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>8664266</v>
       </c>
@@ -2936,7 +4404,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>8666303</v>
       </c>
@@ -2950,7 +4418,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>8687072</v>
       </c>
@@ -2964,7 +4432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>8697536</v>
       </c>
@@ -2978,7 +4446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>8717421</v>
       </c>
@@ -2992,7 +4460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>8723551</v>
       </c>
@@ -3006,7 +4474,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>8734298</v>
       </c>
@@ -3020,7 +4488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>8766117</v>
       </c>
@@ -3034,7 +4502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>8791550</v>
       </c>
@@ -3048,7 +4516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>8837927</v>
       </c>
@@ -3062,7 +4530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>8847103</v>
       </c>
@@ -3076,7 +4544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>8864910</v>
       </c>
@@ -3090,7 +4558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>8920727</v>
       </c>
@@ -3104,7 +4572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>8931170</v>
       </c>
@@ -3118,7 +4586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>8931305</v>
       </c>
@@ -3132,7 +4600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>8958140</v>
       </c>
@@ -3146,7 +4614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>8976584</v>
       </c>
@@ -3160,7 +4628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>9014200</v>
       </c>
@@ -3174,7 +4642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>9020776</v>
       </c>
@@ -3188,7 +4656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>9043600</v>
       </c>
@@ -3202,7 +4670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>9049401</v>
       </c>
@@ -3216,7 +4684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>9063971</v>
       </c>
@@ -3230,7 +4698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>9086188</v>
       </c>
@@ -3244,7 +4712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>9115352</v>
       </c>
@@ -3258,7 +4726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>9118382</v>
       </c>
@@ -3272,7 +4740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>9136320</v>
       </c>
@@ -3286,7 +4754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>9145963</v>
       </c>
@@ -3300,7 +4768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>9189512</v>
       </c>

</xml_diff>

<commit_message>
Changed the plots, fixed up empriical prior
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_validation_set.xlsx
+++ b/GHT/ground_truth_detection_pts_validation_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BCB02C-CE23-41B9-92B2-40D158E17559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD667295-A964-41F5-A84B-0FE9FB1FFD3E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="1190" windowWidth="24220" windowHeight="17910" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
+    <workbookView xWindow="7190" yWindow="810" windowWidth="24220" windowHeight="17910" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ground Truth Points" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,14 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Ground Truth Points'!$B$3:$B$102</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Ground Truth Points'!$C$3:$C$102</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Ground Truth Points'!$M$25</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Ground Truth Points'!$N$25</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Ground Truth Points'!$M$25</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Ground Truth Points'!$N$25</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Ground Truth Points'!$M$25</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Ground Truth Points'!$N$25</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Ground Truth Points'!$M$25</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Ground Truth Points'!$M$26:$M$62</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Ground Truth Points'!$N$25</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Ground Truth Points'!$N$26:$N$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>x</t>
   </si>
@@ -83,6 +82,9 @@
   </si>
   <si>
     <t>Mean_z</t>
+  </si>
+  <si>
+    <t>Final Accumulator Distribution</t>
   </si>
 </sst>
 </file>
@@ -134,12 +136,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -276,6 +281,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Ground Truth Points'!$M$26:$M$66</c:f>
@@ -386,6 +405,9 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,40 +488,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>4.4900000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.7639751552795004E-4</c:v>
+                  <c:v>2.385E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.3333333333333297E-3</c:v>
+                  <c:v>9.2499999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.2797858099062903E-2</c:v>
+                  <c:v>2.9499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.0089686098654699E-2</c:v>
+                  <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.12234706616729001</c:v>
+                  <c:v>0.10539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.207792207792207</c:v>
+                  <c:v>0.2044</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.216911764705882</c:v>
+                  <c:v>0.29239999999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.35820895522388002</c:v>
+                  <c:v>0.46200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.57692307692307598</c:v>
+                  <c:v>0.55500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.72727272727272696</c:v>
+                  <c:v>0.75649999999999995</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.875</c:v>
+                  <c:v>0.88280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,6 +673,7 @@
         <c:axId val="478611664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3083,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3092,6 +3118,8 @@
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
     <col min="2" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="54.90625" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -3473,8 +3501,12 @@
       <c r="D24" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>6022046</v>
       </c>
@@ -3971,7 +4003,7 @@
         <v>23</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>4.4900000000000002E-4</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -3991,7 +4023,7 @@
         <v>24</v>
       </c>
       <c r="N50">
-        <v>7.7639751552795004E-4</v>
+        <v>2.385E-3</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
@@ -4011,7 +4043,7 @@
         <v>25</v>
       </c>
       <c r="N51">
-        <v>8.3333333333333297E-3</v>
+        <v>9.2499999999999995E-3</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
@@ -4031,7 +4063,7 @@
         <v>26</v>
       </c>
       <c r="N52">
-        <v>3.2797858099062903E-2</v>
+        <v>2.9499999999999998E-2</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
@@ -4051,7 +4083,7 @@
         <v>27</v>
       </c>
       <c r="N53">
-        <v>6.0089686098654699E-2</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
@@ -4071,7 +4103,7 @@
         <v>28</v>
       </c>
       <c r="N54">
-        <v>0.12234706616729001</v>
+        <v>0.10539999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
@@ -4091,7 +4123,7 @@
         <v>29</v>
       </c>
       <c r="N55">
-        <v>0.207792207792207</v>
+        <v>0.2044</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
@@ -4111,7 +4143,7 @@
         <v>30</v>
       </c>
       <c r="N56">
-        <v>0.216911764705882</v>
+        <v>0.29239999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
@@ -4131,7 +4163,7 @@
         <v>31</v>
       </c>
       <c r="N57">
-        <v>0.35820895522388002</v>
+        <v>0.46200000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
@@ -4151,7 +4183,7 @@
         <v>32</v>
       </c>
       <c r="N58">
-        <v>0.57692307692307598</v>
+        <v>0.55500000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -4171,7 +4203,7 @@
         <v>33</v>
       </c>
       <c r="N59">
-        <v>0.72727272727272696</v>
+        <v>0.75649999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
@@ -4191,7 +4223,7 @@
         <v>34</v>
       </c>
       <c r="N60">
-        <v>0.875</v>
+        <v>0.88280000000000003</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
@@ -4206,6 +4238,12 @@
       </c>
       <c r="D61">
         <v>18</v>
+      </c>
+      <c r="M61">
+        <v>35</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
@@ -4786,8 +4824,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F102">
     <sortCondition ref="A70"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="M24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>